<commit_message>
testing xlsx file changes
</commit_message>
<xml_diff>
--- a/Projektplanung.xlsx
+++ b/Projektplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\learning\Weiterbildung\Relationale Datenbanken mit SQL\Abschlussprojekt\SQL-Rechnungsprogramm-Gjoni-Reard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5421F6C7-459E-4CF0-98F7-805B255245F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0D1E26-586E-4C21-9457-A63A5238C869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="4752" windowWidth="23256" windowHeight="13176" xr2:uid="{F9B33170-AAF7-4B35-BECE-784E17671F4A}"/>
   </bookViews>
@@ -1369,7 +1369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5967EC-939C-45E1-A30B-BF7CDB6573C3}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>

</xml_diff>